<commit_message>
Subida plantilla fase 3 actualizada
</commit_message>
<xml_diff>
--- a/Fase 3/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 3.xlsx
+++ b/Fase 3/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abelx\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DUOC UC\1. DUOC UC - 2025 II\Capstone\Rúbrica Evaluación - PTY4614-008D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E035B390-EF08-486F-B151-1C14983650CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800672C5-DF6D-4DBC-B11D-7CA05B9D5685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUACION FASE 3" sheetId="1" r:id="rId1"/>
@@ -50,23 +50,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
   <si>
     <t>INTEGRANTES</t>
   </si>
@@ -111,12 +100,6 @@
   </si>
   <si>
     <t>COMISION 1</t>
-  </si>
-  <si>
-    <t>COMISION 2</t>
-  </si>
-  <si>
-    <t>COMISION 3</t>
   </si>
   <si>
     <t>Indicador de Evaluación</t>
@@ -282,21 +265,31 @@
     <t>Muy Relevante</t>
   </si>
   <si>
-    <t>Alexander Hernández</t>
+    <t>Nota Final Comisión</t>
   </si>
   <si>
-    <t>Álvaro Muñoz</t>
+    <t>Nota Juan Gana</t>
   </si>
   <si>
-    <t>Abel Sánchez</t>
+    <t>Nota Alexis Curiche</t>
+  </si>
+  <si>
+    <t>HERNANDEZ OSORIO ALEXANDER IGNACIO</t>
+  </si>
+  <si>
+    <t>MUNOZ PARADA ALVARO ERIK</t>
+  </si>
+  <si>
+    <t>SANCHEZ JIMENEZ ABEL ALONSO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -309,42 +302,50 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -400,7 +401,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +442,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -727,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -765,9 +772,6 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -833,7 +837,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -850,7 +856,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -878,6 +884,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,9 +920,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -953,7 +960,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1059,7 +1066,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1201,7 +1208,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1211,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K797"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1221,8 +1228,10 @@
     <col min="2" max="2" width="66.85546875" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
@@ -1230,13 +1239,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="29">
+      <c r="C2" s="28">
         <v>0.7</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>0.3</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1244,148 +1253,215 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>3</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="31">
+      <c r="B4" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="30">
         <f>C21</f>
-        <v>7</v>
-      </c>
-      <c r="D4" s="37">
-        <f>C60</f>
-        <v>7</v>
-      </c>
-      <c r="E4" s="36">
+        <v>5.4</v>
+      </c>
+      <c r="D4" s="36">
+        <f>H4</f>
+        <v>5</v>
+      </c>
+      <c r="E4" s="35">
         <f>C4*C$2+D4*D$2</f>
-        <v>7</v>
+        <v>5.2799999999999994</v>
+      </c>
+      <c r="F4" s="38">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G4" s="38">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H4" s="59">
+        <f>AVERAGE(F4:G4)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="31">
+      <c r="B5" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="30">
         <f>C34</f>
-        <v>7</v>
-      </c>
-      <c r="D5" s="37">
-        <f>C73</f>
-        <v>7</v>
-      </c>
-      <c r="E5" s="36">
-        <f t="shared" ref="E5:E6" si="0">C5*C$2+D5*D$2</f>
-        <v>7</v>
+        <v>5.4</v>
+      </c>
+      <c r="D5" s="36">
+        <f>H5</f>
+        <v>5</v>
+      </c>
+      <c r="E5" s="35">
+        <f>C5*C$2+D5*D$2</f>
+        <v>5.2799999999999994</v>
+      </c>
+      <c r="F5" s="38">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G5" s="38">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H5" s="59">
+        <f t="shared" ref="H5:H7" si="0">AVERAGE(F5:G5)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="31">
-        <f>C47</f>
+      <c r="B6" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="30">
+        <f>+C47</f>
+        <v>6</v>
+      </c>
+      <c r="D6" s="36">
+        <f>H6</f>
+        <v>5.45</v>
+      </c>
+      <c r="E6" s="35">
+        <f t="shared" ref="E6:E7" si="1">C6*C$2+D6*D$2</f>
+        <v>5.8349999999999991</v>
+      </c>
+      <c r="F6" s="38">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G6" s="38">
+        <v>6</v>
+      </c>
+      <c r="H6" s="59">
+        <f t="shared" si="0"/>
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="30">
+        <f>+C60</f>
         <v>7</v>
       </c>
-      <c r="D6" s="37">
-        <f>C86</f>
-        <v>7</v>
-      </c>
-      <c r="E6" s="36">
+      <c r="D7" s="36">
+        <f t="shared" ref="D5:D7" si="2">C63</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="35">
+        <f t="shared" si="1"/>
+        <v>4.8999999999999995</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0</v>
+      </c>
+      <c r="G7" s="38">
+        <v>0</v>
+      </c>
+      <c r="H7" s="38">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="11" t="str">
         <f>B4</f>
-        <v>Alexander Hernández</v>
-      </c>
-      <c r="C11" s="43" t="s">
+        <v>HERNANDEZ OSORIO ALEXANDER IGNACIO</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
     </row>
     <row r="12" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="44" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="44" t="s">
+      <c r="E12" s="47"/>
+      <c r="F12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="46"/>
-      <c r="H12" s="47" t="s">
+      <c r="G12" s="47"/>
+      <c r="H12" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="46"/>
-      <c r="J12" s="44" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="46"/>
+      <c r="K12" s="47"/>
     </row>
     <row r="13" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="19" t="str">
+      <c r="A13" s="42"/>
+      <c r="B13" s="18" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>8</v>
+      <c r="C13" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D13" s="12" t="str">
-        <f t="shared" ref="D13:D17" si="1">IF($C13=CL,"X","")</f>
+        <f t="shared" ref="D13:D17" si="3">IF($C13=CL,"X","")</f>
+        <v/>
+      </c>
+      <c r="E13" s="12" t="str">
+        <f>IF(D13="X",100*0.15,"")</f>
+        <v/>
+      </c>
+      <c r="F13" s="12" t="str">
+        <f t="shared" ref="F13:F17" si="4">IF($C13=L,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E13" s="12">
-        <f>IF(D13="X",100*0.15,"")</f>
-        <v>15</v>
-      </c>
-      <c r="F13" s="12" t="str">
-        <f t="shared" ref="F13:F17" si="2">IF($C13=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G13" s="12" t="str">
+      <c r="G13" s="12">
         <f>IF(F13="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H13" s="12" t="str">
-        <f t="shared" ref="H13:H17" si="3">IF($C13=ML,"X","")</f>
+        <f t="shared" ref="H13:H17" si="5">IF($C13=ML,"X","")</f>
         <v/>
       </c>
       <c r="I13" s="12" t="str">
@@ -1393,41 +1469,41 @@
         <v/>
       </c>
       <c r="J13" s="12" t="str">
-        <f t="shared" ref="J13:J17" si="4">IF($C13=NL,"X","")</f>
+        <f t="shared" ref="J13:J17" si="6">IF($C13=NL,"X","")</f>
         <v/>
       </c>
       <c r="K13" s="12" t="str">
-        <f t="shared" ref="K13:K17" si="5">IF($J13="X",0,"")</f>
+        <f t="shared" ref="K13:K17" si="7">IF($J13="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:11" ht="26.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="19" t="str">
+      <c r="A14" s="42"/>
+      <c r="B14" s="18" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>8</v>
+      <c r="C14" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D14" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E14" s="12" t="str">
+        <f>IF(D14="X",100*0.25,"")</f>
+        <v/>
+      </c>
+      <c r="F14" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>X</v>
       </c>
-      <c r="E14" s="12">
-        <f>IF(D14="X",100*0.25,"")</f>
-        <v>25</v>
-      </c>
-      <c r="F14" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G14" s="12" t="str">
+      <c r="G14" s="12">
         <f>IF(F14="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H14" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I14" s="12" t="str">
@@ -1435,25 +1511,25 @@
         <v/>
       </c>
       <c r="J14" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K14" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="19" t="str">
+      <c r="A15" s="42"/>
+      <c r="B15" s="18" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>X</v>
       </c>
       <c r="E15" s="12">
@@ -1461,7 +1537,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G15" s="12" t="str">
@@ -1469,7 +1545,7 @@
         <v/>
       </c>
       <c r="H15" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I15" s="12" t="str">
@@ -1477,25 +1553,25 @@
         <v/>
       </c>
       <c r="J15" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K15" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="19" t="str">
+      <c r="A16" s="42"/>
+      <c r="B16" s="18" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>X</v>
       </c>
       <c r="E16" s="12">
@@ -1503,7 +1579,7 @@
         <v>5</v>
       </c>
       <c r="F16" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G16" s="12" t="str">
@@ -1511,7 +1587,7 @@
         <v/>
       </c>
       <c r="H16" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I16" s="12" t="str">
@@ -1519,41 +1595,41 @@
         <v/>
       </c>
       <c r="J16" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K16" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="19" t="str">
+      <c r="A17" s="42"/>
+      <c r="B17" s="18" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>8</v>
+      <c r="C17" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D17" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E17" s="12" t="str">
+        <f>IF(D17="X",100*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="F17" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>X</v>
       </c>
-      <c r="E17" s="12">
-        <f>IF(D17="X",100*0.05,"")</f>
-        <v>5</v>
-      </c>
-      <c r="F17" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G17" s="12" t="str">
+      <c r="G17" s="12">
         <f>IF(F17="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H17" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I17" s="12" t="str">
@@ -1561,21 +1637,21 @@
         <v/>
       </c>
       <c r="J17" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K17" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:11" ht="36" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="19" t="str">
+      <c r="A18" s="42"/>
+      <c r="B18" s="18" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="12" t="str">
@@ -1607,34 +1683,34 @@
         <v/>
       </c>
       <c r="K18" s="12" t="str">
-        <f t="shared" ref="K18:K19" si="6">IF($J18="X",0,"")</f>
+        <f t="shared" ref="K18:K19" si="8">IF($J18="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="19" t="str">
+      <c r="A19" s="42"/>
+      <c r="B19" s="18" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>8</v>
+      <c r="C19" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D19" s="12" t="str">
         <f>IF($C19=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E19" s="12">
+        <v/>
+      </c>
+      <c r="E19" s="12" t="str">
         <f>IF(D19="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F19" s="12" t="str">
         <f>IF($C19=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G19" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G19" s="12">
         <f>IF(F19="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H19" s="12" t="str">
         <f>IF($C19=ML,"X","")</f>
@@ -1649,28 +1725,28 @@
         <v/>
       </c>
       <c r="K19" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
-      <c r="B20" s="18" t="s">
+      <c r="A20" s="41"/>
+      <c r="B20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <f>E20+G20+I20+K20</f>
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13">
         <f>SUM(E13:E19)</f>
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13">
         <f>SUM(G13:G19)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="13">
@@ -1684,89 +1760,89 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
-      <c r="B21" s="21" t="s">
+      <c r="A21" s="43"/>
+      <c r="B21" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="14">
         <f>VLOOKUP(C20,ESCALA_IEP!A2:B202,2,FALSE)</f>
-        <v>7</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="11" t="str">
         <f>B5</f>
-        <v>Álvaro Muñoz</v>
-      </c>
-      <c r="C24" s="43" t="s">
+        <v>MUNOZ PARADA ALVARO ERIK</v>
+      </c>
+      <c r="C24" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="47"/>
     </row>
     <row r="25" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="44" t="s">
+      <c r="C25" s="43"/>
+      <c r="D25" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="44" t="s">
+      <c r="E25" s="47"/>
+      <c r="F25" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="46"/>
-      <c r="H25" s="47" t="s">
+      <c r="G25" s="47"/>
+      <c r="H25" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="46"/>
-      <c r="J25" s="44" t="s">
+      <c r="I25" s="47"/>
+      <c r="J25" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="K25" s="46"/>
+      <c r="K25" s="47"/>
     </row>
     <row r="26" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="19" t="str">
+      <c r="A26" s="42"/>
+      <c r="B26" s="18" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>8</v>
+      <c r="C26" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D26" s="12" t="str">
-        <f t="shared" ref="D26:D30" si="7">IF($C26=CL,"X","")</f>
+        <f t="shared" ref="D26:D30" si="9">IF($C26=CL,"X","")</f>
+        <v/>
+      </c>
+      <c r="E26" s="12" t="str">
+        <f>IF(D26="X",100*0.15,"")</f>
+        <v/>
+      </c>
+      <c r="F26" s="12" t="str">
+        <f t="shared" ref="F26:F30" si="10">IF($C26=L,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E26" s="12">
-        <f>IF(D26="X",100*0.15,"")</f>
-        <v>15</v>
-      </c>
-      <c r="F26" s="12" t="str">
-        <f t="shared" ref="F26:F30" si="8">IF($C26=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G26" s="12" t="str">
+      <c r="G26" s="12">
         <f>IF(F26="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H26" s="12" t="str">
-        <f t="shared" ref="H26:H30" si="9">IF($C26=ML,"X","")</f>
+        <f t="shared" ref="H26:H30" si="11">IF($C26=ML,"X","")</f>
         <v/>
       </c>
       <c r="I26" s="12" t="str">
@@ -1774,41 +1850,41 @@
         <v/>
       </c>
       <c r="J26" s="12" t="str">
-        <f t="shared" ref="J26:J30" si="10">IF($C26=NL,"X","")</f>
+        <f t="shared" ref="J26:J30" si="12">IF($C26=NL,"X","")</f>
         <v/>
       </c>
       <c r="K26" s="12" t="str">
-        <f t="shared" ref="K26:K32" si="11">IF($J26="X",0,"")</f>
+        <f t="shared" ref="K26:K32" si="13">IF($J26="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="19" t="str">
+      <c r="A27" s="42"/>
+      <c r="B27" s="18" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>8</v>
+      <c r="C27" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D27" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E27" s="12" t="str">
+        <f>IF(D27="X",100*0.25,"")</f>
+        <v/>
+      </c>
+      <c r="F27" s="12" t="str">
+        <f t="shared" si="10"/>
         <v>X</v>
       </c>
-      <c r="E27" s="12">
-        <f>IF(D27="X",100*0.25,"")</f>
-        <v>25</v>
-      </c>
-      <c r="F27" s="12" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G27" s="12" t="str">
+      <c r="G27" s="12">
         <f>IF(F27="X",60*0.25,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H27" s="12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="I27" s="12" t="str">
@@ -1816,25 +1892,25 @@
         <v/>
       </c>
       <c r="J27" s="12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K27" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="19" t="str">
+      <c r="A28" s="42"/>
+      <c r="B28" s="18" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>X</v>
       </c>
       <c r="E28" s="12">
@@ -1842,7 +1918,7 @@
         <v>20</v>
       </c>
       <c r="F28" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="G28" s="12" t="str">
@@ -1850,7 +1926,7 @@
         <v/>
       </c>
       <c r="H28" s="12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="I28" s="12" t="str">
@@ -1858,25 +1934,25 @@
         <v/>
       </c>
       <c r="J28" s="12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K28" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="19" t="str">
+      <c r="A29" s="42"/>
+      <c r="B29" s="18" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>X</v>
       </c>
       <c r="E29" s="12">
@@ -1884,7 +1960,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="G29" s="12" t="str">
@@ -1892,7 +1968,7 @@
         <v/>
       </c>
       <c r="H29" s="12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="I29" s="12" t="str">
@@ -1900,41 +1976,41 @@
         <v/>
       </c>
       <c r="J29" s="12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K29" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="19" t="str">
+      <c r="A30" s="42"/>
+      <c r="B30" s="18" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>8</v>
+      <c r="C30" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D30" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E30" s="12" t="str">
+        <f>IF(D30="X",100*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="F30" s="12" t="str">
+        <f t="shared" si="10"/>
         <v>X</v>
       </c>
-      <c r="E30" s="12">
-        <f>IF(D30="X",100*0.05,"")</f>
-        <v>5</v>
-      </c>
-      <c r="F30" s="12" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G30" s="12" t="str">
+      <c r="G30" s="12">
         <f>IF(F30="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H30" s="12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="I30" s="12" t="str">
@@ -1942,21 +2018,21 @@
         <v/>
       </c>
       <c r="J30" s="12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K30" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="19" t="str">
+      <c r="A31" s="42"/>
+      <c r="B31" s="18" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="12" t="str">
@@ -1988,34 +2064,34 @@
         <v/>
       </c>
       <c r="K31" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="19" t="str">
+      <c r="A32" s="42"/>
+      <c r="B32" s="18" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>8</v>
+      <c r="C32" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D32" s="12" t="str">
         <f>IF($C32=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E32" s="12">
+        <v/>
+      </c>
+      <c r="E32" s="12" t="str">
         <f>IF(D32="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F32" s="12" t="str">
         <f>IF($C32=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G32" s="12" t="str">
+        <v>X</v>
+      </c>
+      <c r="G32" s="12">
         <f>IF(F32="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H32" s="12" t="str">
         <f>IF($C32=ML,"X","")</f>
@@ -2030,28 +2106,28 @@
         <v/>
       </c>
       <c r="K32" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
-      <c r="B33" s="18" t="s">
+      <c r="A33" s="41"/>
+      <c r="B33" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="21">
         <f>E33+G33+I33+K33</f>
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="13">
         <f>SUM(E26:E32)</f>
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13">
         <f>SUM(G26:G32)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="13">
@@ -2065,89 +2141,89 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="21" t="s">
+      <c r="A34" s="43"/>
+      <c r="B34" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="14">
         <f>VLOOKUP(C33,ESCALA_IEP!A15:B215,2,FALSE)</f>
-        <v>7</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="11" t="str">
         <f>B6</f>
-        <v>Abel Sánchez</v>
-      </c>
-      <c r="C37" s="43" t="s">
+        <v>SANCHEZ JIMENEZ ABEL ALONSO</v>
+      </c>
+      <c r="C37" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="44" t="s">
+      <c r="D37" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="47"/>
     </row>
     <row r="38" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="44" t="s">
+      <c r="C38" s="43"/>
+      <c r="D38" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="46"/>
-      <c r="F38" s="44" t="s">
+      <c r="E38" s="47"/>
+      <c r="F38" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="46"/>
-      <c r="H38" s="47" t="s">
+      <c r="G38" s="47"/>
+      <c r="H38" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="46"/>
-      <c r="J38" s="44" t="s">
+      <c r="I38" s="47"/>
+      <c r="J38" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="K38" s="46"/>
+      <c r="K38" s="47"/>
     </row>
     <row r="39" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="19" t="str">
+      <c r="A39" s="42"/>
+      <c r="B39" s="18" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>8</v>
+      <c r="C39" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D39" s="12" t="str">
-        <f t="shared" ref="D39:D43" si="12">IF($C39=CL,"X","")</f>
+        <f t="shared" ref="D39:D43" si="14">IF($C39=CL,"X","")</f>
+        <v/>
+      </c>
+      <c r="E39" s="12" t="str">
+        <f>IF(D39="X",100*0.15,"")</f>
+        <v/>
+      </c>
+      <c r="F39" s="12" t="str">
+        <f t="shared" ref="F39:F43" si="15">IF($C39=L,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E39" s="12">
-        <f>IF(D39="X",100*0.15,"")</f>
-        <v>15</v>
-      </c>
-      <c r="F39" s="12" t="str">
-        <f t="shared" ref="F39:F43" si="13">IF($C39=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G39" s="12" t="str">
+      <c r="G39" s="12">
         <f>IF(F39="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H39" s="12" t="str">
-        <f t="shared" ref="H39:H43" si="14">IF($C39=ML,"X","")</f>
+        <f t="shared" ref="H39:H43" si="16">IF($C39=ML,"X","")</f>
         <v/>
       </c>
       <c r="I39" s="12" t="str">
@@ -2155,25 +2231,25 @@
         <v/>
       </c>
       <c r="J39" s="12" t="str">
-        <f t="shared" ref="J39:J43" si="15">IF($C39=NL,"X","")</f>
+        <f t="shared" ref="J39:J43" si="17">IF($C39=NL,"X","")</f>
         <v/>
       </c>
       <c r="K39" s="12" t="str">
-        <f t="shared" ref="K39:K45" si="16">IF($J39="X",0,"")</f>
+        <f t="shared" ref="K39:K45" si="18">IF($J39="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="41"/>
-      <c r="B40" s="19" t="str">
+      <c r="A40" s="42"/>
+      <c r="B40" s="18" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>X</v>
       </c>
       <c r="E40" s="12">
@@ -2181,7 +2257,7 @@
         <v>25</v>
       </c>
       <c r="F40" s="12" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G40" s="12" t="str">
@@ -2189,7 +2265,7 @@
         <v/>
       </c>
       <c r="H40" s="12" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I40" s="12" t="str">
@@ -2197,41 +2273,41 @@
         <v/>
       </c>
       <c r="J40" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K40" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="41"/>
-      <c r="B41" s="19" t="str">
+      <c r="A41" s="42"/>
+      <c r="B41" s="18" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>8</v>
+      <c r="C41" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="D41" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="E41" s="12" t="str">
+        <f>IF(D41="X",100*0.2,"")</f>
+        <v/>
+      </c>
+      <c r="F41" s="12" t="str">
+        <f t="shared" si="15"/>
         <v>X</v>
       </c>
-      <c r="E41" s="12">
-        <f>IF(D41="X",100*0.2,"")</f>
-        <v>20</v>
-      </c>
-      <c r="F41" s="12" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G41" s="12" t="str">
+      <c r="G41" s="12">
         <f>IF(F41="X",60*0.2,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="H41" s="12" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I41" s="12" t="str">
@@ -2239,25 +2315,25 @@
         <v/>
       </c>
       <c r="J41" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K41" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
-      <c r="B42" s="19" t="str">
+      <c r="A42" s="42"/>
+      <c r="B42" s="18" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>X</v>
       </c>
       <c r="E42" s="12">
@@ -2265,7 +2341,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="12" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G42" s="12" t="str">
@@ -2273,7 +2349,7 @@
         <v/>
       </c>
       <c r="H42" s="12" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I42" s="12" t="str">
@@ -2281,25 +2357,25 @@
         <v/>
       </c>
       <c r="J42" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K42" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="19" t="str">
+      <c r="A43" s="42"/>
+      <c r="B43" s="18" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>X</v>
       </c>
       <c r="E43" s="12">
@@ -2307,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="F43" s="12" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G43" s="12" t="str">
@@ -2315,7 +2391,7 @@
         <v/>
       </c>
       <c r="H43" s="12" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I43" s="12" t="str">
@@ -2323,21 +2399,21 @@
         <v/>
       </c>
       <c r="J43" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K43" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="19" t="str">
+      <c r="A44" s="42"/>
+      <c r="B44" s="18" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="12" t="str">
@@ -2369,17 +2445,17 @@
         <v/>
       </c>
       <c r="K44" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
-      <c r="B45" s="19" t="str">
+      <c r="A45" s="42"/>
+      <c r="B45" s="18" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="12" t="str">
@@ -2411,28 +2487,28 @@
         <v/>
       </c>
       <c r="K45" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
-      <c r="B46" s="18" t="s">
+      <c r="A46" s="41"/>
+      <c r="B46" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="21">
         <f>E46+G46+I46+K46</f>
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="13">
         <f>SUM(E39:E45)</f>
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13">
         <f>SUM(G39:G45)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="13">
@@ -2446,73 +2522,73 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="42"/>
-      <c r="B47" s="21" t="s">
+      <c r="A47" s="43"/>
+      <c r="B47" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="14">
         <f>VLOOKUP(C46,ESCALA_IEP!A28:B228,2,FALSE)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="11" t="str">
-        <f>B4</f>
-        <v>Alexander Hernández</v>
-      </c>
-      <c r="C50" s="43" t="s">
+      <c r="B50" s="11">
+        <f>+B7</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="44" t="s">
+      <c r="D50" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="47"/>
     </row>
     <row r="51" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="40"/>
+      <c r="A51" s="41"/>
       <c r="B51" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="44" t="s">
+      <c r="C51" s="43"/>
+      <c r="D51" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="46"/>
-      <c r="F51" s="44" t="s">
+      <c r="E51" s="47"/>
+      <c r="F51" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G51" s="46"/>
-      <c r="H51" s="47" t="s">
+      <c r="G51" s="47"/>
+      <c r="H51" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="I51" s="46"/>
-      <c r="J51" s="44" t="s">
+      <c r="I51" s="47"/>
+      <c r="J51" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="K51" s="46"/>
+      <c r="K51" s="47"/>
     </row>
     <row r="52" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="41"/>
-      <c r="B52" s="19" t="str">
+      <c r="A52" s="42"/>
+      <c r="B52" s="18" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D52" s="12" t="str">
-        <f t="shared" ref="D52:D56" si="17">IF($C52=CL,"X","")</f>
+        <f t="shared" ref="D52:D56" si="19">IF($C52=CL,"X","")</f>
         <v>X</v>
       </c>
       <c r="E52" s="12">
@@ -2520,7 +2596,7 @@
         <v>15</v>
       </c>
       <c r="F52" s="12" t="str">
-        <f t="shared" ref="F52:F56" si="18">IF($C52=L,"X","")</f>
+        <f t="shared" ref="F52:F56" si="20">IF($C52=L,"X","")</f>
         <v/>
       </c>
       <c r="G52" s="12" t="str">
@@ -2528,7 +2604,7 @@
         <v/>
       </c>
       <c r="H52" s="12" t="str">
-        <f t="shared" ref="H52:H56" si="19">IF($C52=ML,"X","")</f>
+        <f t="shared" ref="H52:H56" si="21">IF($C52=ML,"X","")</f>
         <v/>
       </c>
       <c r="I52" s="12" t="str">
@@ -2536,25 +2612,25 @@
         <v/>
       </c>
       <c r="J52" s="12" t="str">
-        <f t="shared" ref="J52:J56" si="20">IF($C52=NL,"X","")</f>
+        <f t="shared" ref="J52:J56" si="22">IF($C52=NL,"X","")</f>
         <v/>
       </c>
       <c r="K52" s="12" t="str">
-        <f t="shared" ref="K52:K58" si="21">IF($J52="X",0,"")</f>
+        <f t="shared" ref="K52:K58" si="23">IF($J52="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="41"/>
-      <c r="B53" s="19" t="str">
+      <c r="A53" s="42"/>
+      <c r="B53" s="18" t="str">
         <f>RUBRICA!A5</f>
         <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D53" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>X</v>
       </c>
       <c r="E53" s="12">
@@ -2562,7 +2638,7 @@
         <v>25</v>
       </c>
       <c r="F53" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="G53" s="12" t="str">
@@ -2570,7 +2646,7 @@
         <v/>
       </c>
       <c r="H53" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="I53" s="12" t="str">
@@ -2578,25 +2654,25 @@
         <v/>
       </c>
       <c r="J53" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="K53" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="41"/>
-      <c r="B54" s="19" t="str">
+      <c r="A54" s="42"/>
+      <c r="B54" s="18" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>X</v>
       </c>
       <c r="E54" s="12">
@@ -2604,7 +2680,7 @@
         <v>20</v>
       </c>
       <c r="F54" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="G54" s="12" t="str">
@@ -2612,7 +2688,7 @@
         <v/>
       </c>
       <c r="H54" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="I54" s="12" t="str">
@@ -2620,25 +2696,25 @@
         <v/>
       </c>
       <c r="J54" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="K54" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="41"/>
-      <c r="B55" s="19" t="str">
+      <c r="A55" s="42"/>
+      <c r="B55" s="18" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D55" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>X</v>
       </c>
       <c r="E55" s="12">
@@ -2646,7 +2722,7 @@
         <v>5</v>
       </c>
       <c r="F55" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="G55" s="12" t="str">
@@ -2654,7 +2730,7 @@
         <v/>
       </c>
       <c r="H55" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="I55" s="12" t="str">
@@ -2662,25 +2738,25 @@
         <v/>
       </c>
       <c r="J55" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="K55" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="41"/>
-      <c r="B56" s="19" t="str">
+      <c r="A56" s="42"/>
+      <c r="B56" s="18" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>X</v>
       </c>
       <c r="E56" s="12">
@@ -2688,7 +2764,7 @@
         <v>5</v>
       </c>
       <c r="F56" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="G56" s="12" t="str">
@@ -2696,7 +2772,7 @@
         <v/>
       </c>
       <c r="H56" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="I56" s="12" t="str">
@@ -2704,21 +2780,21 @@
         <v/>
       </c>
       <c r="J56" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="K56" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="41"/>
-      <c r="B57" s="19" t="str">
+      <c r="A57" s="42"/>
+      <c r="B57" s="18" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="12" t="str">
@@ -2750,17 +2826,17 @@
         <v/>
       </c>
       <c r="K57" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="41"/>
-      <c r="B58" s="19" t="str">
+      <c r="A58" s="42"/>
+      <c r="B58" s="18" t="str">
         <f>RUBRICA!A10</f>
         <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="12" t="str">
@@ -2792,16 +2868,16 @@
         <v/>
       </c>
       <c r="K58" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="40"/>
-      <c r="B59" s="18" t="s">
+      <c r="A59" s="41"/>
+      <c r="B59" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="22">
+      <c r="C59" s="21">
         <f>E59+G59+I59+K59</f>
         <v>100</v>
       </c>
@@ -2827,8 +2903,8 @@
       </c>
     </row>
     <row r="60" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="42"/>
-      <c r="B60" s="21" t="s">
+      <c r="A60" s="43"/>
+      <c r="B60" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C60" s="14">
@@ -2839,764 +2915,276 @@
     <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B63" s="11" t="str">
-        <f>B5</f>
-        <v>Álvaro Muñoz</v>
-      </c>
-      <c r="C63" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="45"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="46"/>
+      <c r="A63" s="49"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="47"/>
     </row>
     <row r="64" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
-      <c r="B64" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="46"/>
-      <c r="F64" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="G64" s="46"/>
-      <c r="H64" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="I64" s="46"/>
-      <c r="J64" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="K64" s="46"/>
+      <c r="A64" s="41"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="47"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="47"/>
     </row>
     <row r="65" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="41"/>
-      <c r="B65" s="19" t="str">
-        <f>RUBRICA!A4</f>
-        <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="12" t="str">
-        <f t="shared" ref="D65:D69" si="22">IF($C65=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E65" s="12">
-        <f>IF(D65="X",100*0.15,"")</f>
-        <v>15</v>
-      </c>
-      <c r="F65" s="12" t="str">
-        <f t="shared" ref="F65:F69" si="23">IF($C65=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G65" s="12" t="str">
-        <f>IF(F65="X",60*0.15,"")</f>
-        <v/>
-      </c>
-      <c r="H65" s="12" t="str">
-        <f t="shared" ref="H65:H69" si="24">IF($C65=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I65" s="12" t="str">
-        <f>IF(H65="X",30*0.15,"")</f>
-        <v/>
-      </c>
-      <c r="J65" s="12" t="str">
-        <f t="shared" ref="J65:J69" si="25">IF($C65=NL,"X","")</f>
-        <v/>
-      </c>
-      <c r="K65" s="12" t="str">
-        <f t="shared" ref="K65:K71" si="26">IF($J65="X",0,"")</f>
-        <v/>
-      </c>
+      <c r="A65" s="42"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
     </row>
     <row r="66" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
-      <c r="B66" s="19" t="str">
-        <f>RUBRICA!A5</f>
-        <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v>X</v>
-      </c>
-      <c r="E66" s="12">
-        <f>IF(D66="X",100*0.25,"")</f>
-        <v>25</v>
-      </c>
-      <c r="F66" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="G66" s="12" t="str">
-        <f>IF(F66="X",60*0.25,"")</f>
-        <v/>
-      </c>
-      <c r="H66" s="12" t="str">
-        <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="I66" s="12" t="str">
-        <f>IF(H66="X",30*0.25,"")</f>
-        <v/>
-      </c>
-      <c r="J66" s="12" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="K66" s="12" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
+      <c r="A66" s="42"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
     </row>
     <row r="67" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="41"/>
-      <c r="B67" s="19" t="str">
-        <f>RUBRICA!A6</f>
-        <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v>X</v>
-      </c>
-      <c r="E67" s="12">
-        <f>IF(D67="X",100*0.2,"")</f>
-        <v>20</v>
-      </c>
-      <c r="F67" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="G67" s="12" t="str">
-        <f>IF(F67="X",60*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="H67" s="12" t="str">
-        <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="I67" s="12" t="str">
-        <f>IF(H67="X",30*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="J67" s="12" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="K67" s="12" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
+      <c r="A67" s="42"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
     </row>
     <row r="68" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="41"/>
-      <c r="B68" s="19" t="str">
-        <f>RUBRICA!A7</f>
-        <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v>X</v>
-      </c>
-      <c r="E68" s="12">
-        <f>IF(D68="X",100*0.05,"")</f>
-        <v>5</v>
-      </c>
-      <c r="F68" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="G68" s="12" t="str">
-        <f>IF(F68="X",60*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="H68" s="12" t="str">
-        <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="I68" s="12" t="str">
-        <f>IF(H68="X",30*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="J68" s="12" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="K68" s="12" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
+      <c r="A68" s="42"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
     </row>
     <row r="69" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="41"/>
-      <c r="B69" s="19" t="str">
-        <f>RUBRICA!A8</f>
-        <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v>X</v>
-      </c>
-      <c r="E69" s="12">
-        <f>IF(D69="X",100*0.05,"")</f>
-        <v>5</v>
-      </c>
-      <c r="F69" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="G69" s="12" t="str">
-        <f>IF(F69="X",60*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="H69" s="12" t="str">
-        <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="I69" s="12" t="str">
-        <f>IF(H69="X",30*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="J69" s="12" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="K69" s="12" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
+      <c r="A69" s="42"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
     </row>
     <row r="70" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="41"/>
-      <c r="B70" s="19" t="str">
-        <f>RUBRICA!A9</f>
-        <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="12" t="str">
-        <f>IF($C70=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E70" s="12">
-        <f>IF(D70="X",100*0.2,"")</f>
-        <v>20</v>
-      </c>
-      <c r="F70" s="12" t="str">
-        <f>IF($C70=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G70" s="12" t="str">
-        <f>IF(F70="X",60*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="H70" s="12" t="str">
-        <f>IF($C70=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I70" s="12" t="str">
-        <f>IF(H70="X",30*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="J70" s="12" t="str">
-        <f>IF($C70=NL,"X","")</f>
-        <v/>
-      </c>
-      <c r="K70" s="12" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
+      <c r="A70" s="42"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
     </row>
     <row r="71" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="41"/>
-      <c r="B71" s="19" t="str">
-        <f>RUBRICA!A10</f>
-        <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="12" t="str">
-        <f>IF($C71=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E71" s="12">
-        <f>IF(D71="X",100*0.1,"")</f>
-        <v>10</v>
-      </c>
-      <c r="F71" s="12" t="str">
-        <f>IF($C71=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G71" s="12" t="str">
-        <f>IF(F71="X",60*0.1,"")</f>
-        <v/>
-      </c>
-      <c r="H71" s="12" t="str">
-        <f>IF($C71=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I71" s="12" t="str">
-        <f>IF(H71="X",30*0.1,"")</f>
-        <v/>
-      </c>
-      <c r="J71" s="12" t="str">
-        <f>IF($C71=NL,"X","")</f>
-        <v/>
-      </c>
-      <c r="K71" s="12" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
+      <c r="A71" s="42"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
     </row>
     <row r="72" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="40"/>
-      <c r="B72" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="22">
-        <f>E72+G72+I72+K72</f>
-        <v>100</v>
-      </c>
+      <c r="A72" s="41"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="21"/>
       <c r="D72" s="13"/>
-      <c r="E72" s="13">
-        <f>SUM(E65:E71)</f>
-        <v>100</v>
-      </c>
+      <c r="E72" s="13"/>
       <c r="F72" s="13"/>
-      <c r="G72" s="13">
-        <f>SUM(G65:G71)</f>
-        <v>0</v>
-      </c>
+      <c r="G72" s="13"/>
       <c r="H72" s="13"/>
-      <c r="I72" s="13">
-        <f>SUM(I65:I71)</f>
-        <v>0</v>
-      </c>
+      <c r="I72" s="13"/>
       <c r="J72" s="13"/>
-      <c r="K72" s="13">
-        <f>SUM(K65:K71)</f>
-        <v>0</v>
-      </c>
+      <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="42"/>
-      <c r="B73" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="14">
-        <f>VLOOKUP(C72,ESCALA_IEP!A54:B254,2,FALSE)</f>
-        <v>7</v>
-      </c>
+      <c r="A73" s="43"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="14"/>
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B76" s="11" t="str">
-        <f>B6</f>
-        <v>Abel Sánchez</v>
-      </c>
-      <c r="C76" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" s="45"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="45"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="45"/>
-      <c r="J76" s="45"/>
-      <c r="K76" s="46"/>
+      <c r="A76" s="49"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="46"/>
+      <c r="G76" s="46"/>
+      <c r="H76" s="46"/>
+      <c r="I76" s="46"/>
+      <c r="J76" s="46"/>
+      <c r="K76" s="47"/>
     </row>
     <row r="77" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="40"/>
-      <c r="B77" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="42"/>
-      <c r="D77" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="46"/>
-      <c r="F77" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" s="46"/>
-      <c r="H77" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="I77" s="46"/>
-      <c r="J77" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="K77" s="46"/>
+      <c r="A77" s="41"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="43"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="45"/>
+      <c r="G77" s="47"/>
+      <c r="H77" s="48"/>
+      <c r="I77" s="47"/>
+      <c r="J77" s="45"/>
+      <c r="K77" s="47"/>
     </row>
     <row r="78" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="41"/>
-      <c r="B78" s="19" t="str">
-        <f>RUBRICA!A4</f>
-        <v xml:space="preserve">1. Presenta el proyecto considerando la relevancia, objetivos, metodología y desarrollo, de acuerdo a los estándares de calidad de la disciplina. </v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="12" t="str">
-        <f t="shared" ref="D78:D82" si="27">IF($C78=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E78" s="12">
-        <f>IF(D78="X",100*0.15,"")</f>
-        <v>15</v>
-      </c>
-      <c r="F78" s="12" t="str">
-        <f t="shared" ref="F78:F82" si="28">IF($C78=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G78" s="12" t="str">
-        <f>IF(F78="X",60*0.15,"")</f>
-        <v/>
-      </c>
-      <c r="H78" s="12" t="str">
-        <f t="shared" ref="H78:H82" si="29">IF($C78=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I78" s="12" t="str">
-        <f>IF(H78="X",30*0.15,"")</f>
-        <v/>
-      </c>
-      <c r="J78" s="12" t="str">
-        <f t="shared" ref="J78:J82" si="30">IF($C78=NL,"X","")</f>
-        <v/>
-      </c>
-      <c r="K78" s="12" t="str">
-        <f t="shared" ref="K78:K84" si="31">IF($J78="X",0,"")</f>
-        <v/>
-      </c>
+      <c r="A78" s="42"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
     </row>
     <row r="79" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="41"/>
-      <c r="B79" s="19" t="str">
-        <f>RUBRICA!A5</f>
-        <v xml:space="preserve">2. Presenta las evidencias del Proyecto APT, dando cuenta del cumplimiento de los objetivos y de acuerdo a los estándares de la disciplina. </v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="12" t="str">
-        <f t="shared" si="27"/>
-        <v>X</v>
-      </c>
-      <c r="E79" s="12">
-        <f>IF(D79="X",100*0.25,"")</f>
-        <v>25</v>
-      </c>
-      <c r="F79" s="12" t="str">
-        <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="G79" s="12" t="str">
-        <f>IF(F79="X",60*0.25,"")</f>
-        <v/>
-      </c>
-      <c r="H79" s="12" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="I79" s="12" t="str">
-        <f>IF(H79="X",30*0.25,"")</f>
-        <v/>
-      </c>
-      <c r="J79" s="12" t="str">
-        <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="K79" s="12" t="str">
-        <f t="shared" si="31"/>
-        <v/>
-      </c>
+      <c r="A79" s="42"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
     </row>
     <row r="80" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="41"/>
-      <c r="B80" s="19" t="str">
-        <f>RUBRICA!A6</f>
-        <v>3. Responde las preguntas realizadas por la comisión, cumpliendo con los estándares de calidad de la disciplina.</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" s="12" t="str">
-        <f t="shared" si="27"/>
-        <v>X</v>
-      </c>
-      <c r="E80" s="12">
-        <f>IF(D80="X",100*0.2,"")</f>
-        <v>20</v>
-      </c>
-      <c r="F80" s="12" t="str">
-        <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="G80" s="12" t="str">
-        <f>IF(F80="X",60*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="H80" s="12" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="I80" s="12" t="str">
-        <f>IF(H80="X",30*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="J80" s="12" t="str">
-        <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="K80" s="12" t="str">
-        <f t="shared" si="31"/>
-        <v/>
-      </c>
+      <c r="A80" s="42"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="12"/>
+      <c r="K80" s="12"/>
     </row>
     <row r="81" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="41"/>
-      <c r="B81" s="19" t="str">
-        <f>RUBRICA!A7</f>
-        <v>4. Expone el Proyecto APT, considerando el formato y el tiempo establecido para la presentación.</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" s="12" t="str">
-        <f t="shared" si="27"/>
-        <v>X</v>
-      </c>
-      <c r="E81" s="12">
-        <f>IF(D81="X",100*0.05,"")</f>
-        <v>5</v>
-      </c>
-      <c r="F81" s="12" t="str">
-        <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="G81" s="12" t="str">
-        <f>IF(F81="X",60*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="H81" s="12" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="I81" s="12" t="str">
-        <f>IF(H81="X",30*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="J81" s="12" t="str">
-        <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="K81" s="12" t="str">
-        <f t="shared" si="31"/>
-        <v/>
-      </c>
+      <c r="A81" s="42"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
     </row>
     <row r="82" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="41"/>
-      <c r="B82" s="19" t="str">
-        <f>RUBRICA!A8</f>
-        <v>5. Expresa sus ideas con fluidez, claridad y precisión, utilizando lenguaje técnico propio de la disciplina.</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" s="12" t="str">
-        <f t="shared" si="27"/>
-        <v>X</v>
-      </c>
-      <c r="E82" s="12">
-        <f>IF(D82="X",100*0.05,"")</f>
-        <v>5</v>
-      </c>
-      <c r="F82" s="12" t="str">
-        <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="G82" s="12" t="str">
-        <f>IF(F82="X",60*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="H82" s="12" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="I82" s="12" t="str">
-        <f>IF(H82="X",30*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="J82" s="12" t="str">
-        <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="K82" s="12" t="str">
-        <f t="shared" si="31"/>
-        <v/>
-      </c>
+      <c r="A82" s="42"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
     </row>
     <row r="83" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="41"/>
-      <c r="B83" s="19" t="str">
-        <f>RUBRICA!A9</f>
-        <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estructura y nombres solicitados, guardando todas las evidencias de avances en Git</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="12" t="str">
-        <f>IF($C83=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E83" s="12">
-        <f>IF(D83="X",100*0.2,"")</f>
-        <v>20</v>
-      </c>
-      <c r="F83" s="12" t="str">
-        <f>IF($C83=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G83" s="12" t="str">
-        <f>IF(F83="X",60*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="H83" s="12" t="str">
-        <f>IF($C83=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I83" s="12" t="str">
-        <f>IF(H83="X",30*0.2,"")</f>
-        <v/>
-      </c>
-      <c r="J83" s="12" t="str">
-        <f>IF($C83=NL,"X","")</f>
-        <v/>
-      </c>
-      <c r="K83" s="12" t="str">
-        <f t="shared" si="31"/>
-        <v/>
-      </c>
+      <c r="A83" s="42"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="12"/>
     </row>
     <row r="84" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="41"/>
-      <c r="B84" s="19" t="str">
-        <f>RUBRICA!A10</f>
-        <v xml:space="preserve">7. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. </v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="12" t="str">
-        <f>IF($C84=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E84" s="12">
-        <f>IF(D84="X",100*0.1,"")</f>
-        <v>10</v>
-      </c>
-      <c r="F84" s="12" t="str">
-        <f>IF($C84=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G84" s="12" t="str">
-        <f>IF(F84="X",60*0.1,"")</f>
-        <v/>
-      </c>
-      <c r="H84" s="12" t="str">
-        <f>IF($C84=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I84" s="12" t="str">
-        <f>IF(H84="X",30*0.1,"")</f>
-        <v/>
-      </c>
-      <c r="J84" s="12" t="str">
-        <f>IF($C84=NL,"X","")</f>
-        <v/>
-      </c>
-      <c r="K84" s="12" t="str">
-        <f t="shared" si="31"/>
-        <v/>
-      </c>
+      <c r="A84" s="42"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
     </row>
     <row r="85" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="40"/>
-      <c r="B85" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85" s="22">
-        <f>E85+G85+I85+K85</f>
-        <v>100</v>
-      </c>
+      <c r="A85" s="41"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="21"/>
       <c r="D85" s="13"/>
-      <c r="E85" s="13">
-        <f>SUM(E78:E84)</f>
-        <v>100</v>
-      </c>
+      <c r="E85" s="13"/>
       <c r="F85" s="13"/>
-      <c r="G85" s="13">
-        <f>SUM(G78:G84)</f>
-        <v>0</v>
-      </c>
+      <c r="G85" s="13"/>
       <c r="H85" s="13"/>
-      <c r="I85" s="13">
-        <f>SUM(I78:I84)</f>
-        <v>0</v>
-      </c>
+      <c r="I85" s="13"/>
       <c r="J85" s="13"/>
-      <c r="K85" s="13">
-        <f>SUM(K78:K84)</f>
-        <v>0</v>
-      </c>
+      <c r="K85" s="13"/>
     </row>
     <row r="86" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="42"/>
-      <c r="B86" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C86" s="14">
-        <f>VLOOKUP(C85,ESCALA_IEP!A67:B267,2,FALSE)</f>
-        <v>7</v>
-      </c>
+      <c r="A86" s="43"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="14"/>
     </row>
     <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4311,6 +3899,32 @@
     <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A76:A86"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="A63:A73"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:K63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="A50:A60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="J51:K51"/>
     <mergeCell ref="A11:A21"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D37:K37"/>
@@ -4327,34 +3941,8 @@
     <mergeCell ref="A37:A47"/>
     <mergeCell ref="A24:A34"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A50:A60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="D24:K24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="A63:A73"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:K63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="A76:A86"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:K76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:K77"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:C6">
+  <conditionalFormatting sqref="C4:C7">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>
@@ -4363,7 +3951,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Error de Ingreso - Nota debe estar entre 1,0 y 7,0" sqref="C4:C6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Error de Ingreso - Nota debe estar entre 1,0 y 7,0" sqref="C4:C7" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>7</formula2>
     </dataValidation>
@@ -4404,184 +3992,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="51" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="51"/>
+      <c r="B2" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="49" t="s">
+      <c r="C2" s="55" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="54" t="s">
+      <c r="D2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="E2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="51"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="E3" s="26">
+        <v>0</v>
+      </c>
+      <c r="F3" s="51"/>
+    </row>
+    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="50"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="E3" s="27">
-        <v>0</v>
-      </c>
-      <c r="F3" s="50"/>
-    </row>
-    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="F4" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="136.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="28">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="136.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="F5" s="27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="F6" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="28">
+      <c r="C7" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="23">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="23" t="s">
+    <row r="10" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="24">
+      <c r="F10" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7043,10 +6631,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -9756,8 +9344,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
-        <v>60</v>
+      <c r="A1" s="57" t="s">
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>12</v>
@@ -9767,23 +9355,23 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="38" t="s">
+      <c r="D2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="10">
         <v>4</v>

</xml_diff>